<commit_message>
Final Pengantar SIMALA Dan Template SIHAS
</commit_message>
<xml_diff>
--- a/sihas/template/krs_khs_template.xlsx
+++ b/sihas/template/krs_khs_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740"/>
   </bookViews>
   <sheets>
     <sheet name="KRS" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>SEKOLAH TINGGI MANAJEMEN INFORMATIKA DAN KOMPUTER</t>
   </si>
@@ -90,39 +90,21 @@
     <t>NAMA MATA KULIAH</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>(SKS)</t>
   </si>
   <si>
-    <t>*Coret Salah Satu</t>
-  </si>
-  <si>
     <t>Palu,</t>
   </si>
   <si>
-    <t>1. Mahasiswa (Putih)</t>
-  </si>
-  <si>
     <t>Mengetahui,</t>
   </si>
   <si>
     <t>Mahasiswa,</t>
   </si>
   <si>
-    <t>2. BAAK</t>
-  </si>
-  <si>
     <t>Dosen Wali</t>
   </si>
   <si>
-    <t>3. Prodi</t>
-  </si>
-  <si>
-    <t>4. Dosen Wali</t>
-  </si>
-  <si>
     <t>STMIK ADHI GUNA</t>
   </si>
   <si>
@@ -138,6 +120,9 @@
     <t xml:space="preserve">: </t>
   </si>
   <si>
+    <t>T.A</t>
+  </si>
+  <si>
     <t>N I M</t>
   </si>
   <si>
@@ -147,6 +132,9 @@
     <t>JURUSAN</t>
   </si>
   <si>
+    <t>SMTR.</t>
+  </si>
+  <si>
     <t>SKS</t>
   </si>
   <si>
@@ -156,9 +144,6 @@
     <t>N x K</t>
   </si>
   <si>
-    <t>KET</t>
-  </si>
-  <si>
     <t>JUMLAH</t>
   </si>
   <si>
@@ -183,23 +168,20 @@
     <t>KEPALA BAAK</t>
   </si>
   <si>
-    <t>SMTR</t>
-  </si>
-  <si>
-    <t>TA.</t>
-  </si>
-  <si>
-    <t>MOH. ANDIKA, S.Sos,. M.A.P</t>
+    <t>MOH.ANDIKA,.S.Sos,.M.A.P</t>
   </si>
   <si>
     <t>NIK. 140 201 031</t>
+  </si>
+  <si>
+    <t>* Cetak Tiga Lembar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,13 +190,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Courier New"/>
@@ -265,6 +240,25 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -274,7 +268,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -335,17 +329,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -363,11 +346,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -388,9 +397,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -415,15 +421,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -431,14 +428,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -459,44 +450,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -504,25 +495,76 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -537,6 +579,104 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>475476</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="177800" y="63501"/>
+          <a:ext cx="742176" cy="711200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>46996</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5892800" y="0"/>
+          <a:ext cx="821696" cy="787401"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -826,170 +966,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="26" customWidth="1"/>
-    <col min="3" max="4" width="5" style="26" customWidth="1"/>
-    <col min="5" max="5" width="41.83203125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="5" style="26" customWidth="1"/>
-    <col min="9" max="10" width="6.83203125" style="26" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="5.83203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="20" customWidth="1"/>
+    <col min="3" max="4" width="5" style="20" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="5" style="20" customWidth="1"/>
+    <col min="9" max="10" width="6.83203125" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
     </row>
     <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="42"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="27" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="27" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="24" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="1"/>
@@ -1013,110 +1153,104 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="7" t="s">
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="48" t="s">
+      <c r="H10" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="49"/>
+      <c r="B11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="32"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="53" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>26</v>
+      <c r="G14" s="53" t="s">
+        <v>23</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
+      <c r="A15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="53" t="s">
+        <v>24</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1127,10 +1261,8 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="36"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1141,10 +1273,8 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="36"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1155,13 +1285,13 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1175,45 +1305,53 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C20" s="39"/>
-      <c r="H20" s="39"/>
+      <c r="C20" s="33"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C21" s="39"/>
-      <c r="H21" s="39"/>
+      <c r="C21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C22" s="39"/>
-      <c r="H22" s="39"/>
+      <c r="C22" s="33"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C23" s="39"/>
-      <c r="H23" s="39"/>
+      <c r="C23" s="33"/>
+      <c r="H23" s="33"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C24" s="39"/>
-      <c r="H24" s="39"/>
+      <c r="C24" s="33"/>
+      <c r="H24" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:L11"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="F10:F11"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.70069444444444495" right="0.196527777777778" top="0.196527777777778" bottom="0.16041666666666701" header="0.196527777777778" footer="0.101388888888889"/>
   <pageSetup paperSize="9" orientation="landscape"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1221,188 +1359,194 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="2.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="A3" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+        <v>29</v>
+      </c>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="4" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="23"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="23"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="23"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D9" s="3"/>
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="51"/>
-      <c r="I11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>42</v>
-      </c>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="63"/>
+      <c r="I11" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="63"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="6"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="44"/>
     </row>
     <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="6"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="44"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
@@ -1417,130 +1561,141 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>47</v>
+      <c r="B15" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="66" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20">
+      <c r="C16" s="59"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="16">
         <f>SUM(F12:F13)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="42">
         <f>SUM(F12:F13)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="17">
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="38">
         <f>SUM(I12:I13)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="17" t="e">
-        <f>I16/E16</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
+      <c r="B17" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F18" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="F18" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F19" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="F19" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="F23" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="F24" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="18">
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="A3:I4"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="F15:H15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:H16"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.2" right="0.2" top="0.2" bottom="0.2" header="0.2" footer="0.2"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Perbaikan Layanan KRS SIHAS
</commit_message>
<xml_diff>
--- a/sihas/template/krs_khs_template.xlsx
+++ b/sihas/template/krs_khs_template.xlsx
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -489,43 +489,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -534,38 +498,77 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,7 +970,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -984,93 +987,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
       <c r="M1" s="34"/>
       <c r="N1" s="34"/>
     </row>
     <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
       <c r="M2" s="34"/>
       <c r="N2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
       <c r="M3" s="34"/>
       <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
       <c r="M4" s="35"/>
       <c r="N4" s="35"/>
       <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
     </row>
     <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -1080,19 +1083,19 @@
       <c r="C6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="21" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
@@ -1102,19 +1105,19 @@
       <c r="C7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="21" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -1124,8 +1127,8 @@
       <c r="C8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1168,7 @@
       <c r="F10" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="40" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="49" t="s">
@@ -1180,7 +1183,7 @@
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="49" t="s">
@@ -1188,8 +1191,8 @@
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="51" t="s">
+      <c r="F11" s="51"/>
+      <c r="G11" s="40" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="49"/>
@@ -1233,13 +1236,13 @@
     <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="30"/>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="41" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="53" t="s">
+      <c r="G14" s="41" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="1"/>
@@ -1249,7 +1252,7 @@
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="41" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="1"/>
@@ -1379,54 +1382,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
@@ -1442,16 +1445,16 @@
       <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
       <c r="J6" s="2"/>
       <c r="K6" s="19"/>
     </row>
@@ -1463,16 +1466,16 @@
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
       <c r="J7" s="2"/>
       <c r="K7" s="19"/>
     </row>
@@ -1484,16 +1487,16 @@
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
       <c r="J8" s="2"/>
       <c r="K8" s="19"/>
     </row>
@@ -1501,10 +1504,10 @@
       <c r="D9" s="3"/>
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="49" t="s">
@@ -1512,17 +1515,17 @@
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="62" t="s">
+      <c r="G11" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="63"/>
-      <c r="I11" s="62" t="s">
+      <c r="H11" s="58"/>
+      <c r="I11" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="63"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
@@ -1533,8 +1536,8 @@
       <c r="F12" s="7"/>
       <c r="G12" s="11"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="44"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="63"/>
     </row>
     <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1545,8 +1548,8 @@
       <c r="F13" s="7"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="44"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
@@ -1561,42 +1564,42 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="64" t="s">
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="65" t="s">
+      <c r="F15" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="67" t="s">
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="66" t="s">
+      <c r="J15" s="47" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="16">
         <f>SUM(F12:F13)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="64">
         <f>SUM(F12:F13)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
       <c r="I16" s="38">
         <f>SUM(I12:I13)</f>
         <v>0</v>
@@ -1604,73 +1607,71 @@
       <c r="J16" s="38"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="38"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
       <c r="I17" s="38"/>
       <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E22" s="39"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="55" t="s">
+      <c r="F24" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F16:H16"/>
@@ -1687,6 +1688,8 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.2" right="0.2" top="0.2" bottom="0.2" header="0.2" footer="0.2"/>

</xml_diff>